<commit_message>
Reading Bid opening time in a separate column
</commit_message>
<xml_diff>
--- a/test/data/bids.xlsx
+++ b/test/data/bids.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>processo</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>objeto teste</t>
+  </si>
+  <si>
+    <t>Hora de Abertura</t>
   </si>
 </sst>
 </file>
@@ -127,9 +130,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -478,10 +482,13 @@
     <col min="2" max="2" width="20.25" customWidth="1"/>
     <col min="3" max="3" width="23.875" customWidth="1"/>
     <col min="4" max="4" width="25.125" customWidth="1"/>
-    <col min="5" max="5" width="24.125" customWidth="1"/>
+    <col min="5" max="6" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="11.75" customWidth="1"/>
+    <col min="11" max="11" width="13.625" customWidth="1"/>
+    <col min="12" max="12" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,25 +505,28 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -530,19 +540,22 @@
         <v>3</v>
       </c>
       <c r="E2" s="1">
-        <v>42479.583333333336</v>
-      </c>
-      <c r="F2" t="s">
+        <v>42479.041666666664</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -558,14 +571,17 @@
       <c r="E3" s="1">
         <v>42468.583333333336</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -579,22 +595,25 @@
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>42480.416666666664</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
+        <v>42480.041666666664</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.41666666666666669</v>
       </c>
       <c r="G4" t="s">
         <v>23</v>
       </c>
       <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1234</v>
       </c>
@@ -605,7 +624,10 @@
         <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>29609.849305555555</v>
+        <v>29609.523611111112</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.84930555555555554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting object on bid from column on excel file
</commit_message>
<xml_diff>
--- a/test/data/bids.xlsx
+++ b/test/data/bids.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>processo</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Hora de Abertura</t>
+  </si>
+  <si>
+    <t>Abalone</t>
+  </si>
+  <si>
+    <t>Jiribatuba2</t>
+  </si>
+  <si>
+    <t>Objeto</t>
   </si>
 </sst>
 </file>
@@ -130,10 +139,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -486,9 +496,10 @@
     <col min="10" max="10" width="11.75" customWidth="1"/>
     <col min="11" max="11" width="13.625" customWidth="1"/>
     <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,8 +536,11 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -554,8 +568,11 @@
       <c r="K2" t="s">
         <v>16</v>
       </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -581,7 +598,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -612,8 +629,11 @@
       <c r="K4" t="s">
         <v>19</v>
       </c>
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1234</v>
       </c>
@@ -628,9 +648,13 @@
       </c>
       <c r="F5" s="2">
         <v>0.84930555555555554</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>